<commit_message>
Se puede usar ya en principio y tiene buen formato
</commit_message>
<xml_diff>
--- a/Grados_UGR_Centros.xlsx
+++ b/Grados_UGR_Centros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\SyllaBUG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB69F716-1239-481D-8754-7875994E1054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820A49B6-61D4-449A-957E-C4E936BF0B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="253">
   <si>
     <t>Grado</t>
   </si>
@@ -706,27 +706,6 @@
     <t>Biblioteca</t>
   </si>
   <si>
-    <t>BFA</t>
-  </si>
-  <si>
-    <t>BDE</t>
-  </si>
-  <si>
-    <t>BCPS</t>
-  </si>
-  <si>
-    <t>BBA</t>
-  </si>
-  <si>
-    <t>BCM</t>
-  </si>
-  <si>
-    <t>BDE+BEE</t>
-  </si>
-  <si>
-    <t>BDE+BCPS</t>
-  </si>
-  <si>
     <t>B. Económicas y Empres.</t>
   </si>
   <si>
@@ -761,6 +740,45 @@
   </si>
   <si>
     <t>B. Informática y Telecom.</t>
+  </si>
+  <si>
+    <t>B. Politécnica</t>
+  </si>
+  <si>
+    <t>B. Políticas y Sociolog.</t>
+  </si>
+  <si>
+    <t>B. Educación</t>
+  </si>
+  <si>
+    <t>B. Bellas Artes</t>
+  </si>
+  <si>
+    <t>B. Derecho</t>
+  </si>
+  <si>
+    <t>B. Deporte</t>
+  </si>
+  <si>
+    <t>B. Derecho + B. Económicas y Empres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. Políticas y Sociolog. + </t>
+  </si>
+  <si>
+    <t>B. Derecho + B. Políticas y Sociolog.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. Económicas y Empres. + </t>
+  </si>
+  <si>
+    <t>B. Ciencias + B. Informática y Telecom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B. Informática y Telecom. + B. Económicas y Empres.</t>
+  </si>
+  <si>
+    <t>B. Filosofía y Letras A + B. Eduación</t>
   </si>
 </sst>
 </file>
@@ -1136,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="134" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1167,7 +1185,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1181,7 +1199,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,6 +1212,9 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
+      <c r="D4" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1206,7 +1227,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1220,7 +1241,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1233,6 +1254,9 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
+      <c r="D7" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1245,7 +1269,7 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1255,8 +1279,11 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1266,8 +1293,11 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1280,6 +1310,9 @@
       <c r="C11" t="s">
         <v>28</v>
       </c>
+      <c r="D11" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1291,6 +1324,9 @@
       <c r="C12" t="s">
         <v>31</v>
       </c>
+      <c r="D12" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1302,6 +1338,9 @@
       <c r="C13" t="s">
         <v>34</v>
       </c>
+      <c r="D13" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1313,6 +1352,9 @@
       <c r="C14" t="s">
         <v>36</v>
       </c>
+      <c r="D14" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1324,6 +1366,9 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
+      <c r="D15" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1335,6 +1380,9 @@
       <c r="C16" t="s">
         <v>41</v>
       </c>
+      <c r="D16" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -1346,6 +1394,9 @@
       <c r="C17" t="s">
         <v>44</v>
       </c>
+      <c r="D17" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1357,6 +1408,9 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
+      <c r="D18" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1369,7 +1423,7 @@
         <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1383,7 +1437,7 @@
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1397,7 +1451,7 @@
         <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1411,7 +1465,7 @@
         <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1425,7 +1479,7 @@
         <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1439,7 +1493,7 @@
         <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1453,7 +1507,7 @@
         <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1467,7 +1521,7 @@
         <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1481,7 +1535,7 @@
         <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1495,7 +1549,7 @@
         <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1509,7 +1563,7 @@
         <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1523,7 +1577,7 @@
         <v>72</v>
       </c>
       <c r="D30" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1537,7 +1591,7 @@
         <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1551,7 +1605,7 @@
         <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1565,7 +1619,7 @@
         <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1579,7 +1633,7 @@
         <v>82</v>
       </c>
       <c r="D34" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1593,7 +1647,7 @@
         <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1607,7 +1661,7 @@
         <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1621,7 +1675,7 @@
         <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1635,7 +1689,7 @@
         <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1649,7 +1703,7 @@
         <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1673,6 +1727,9 @@
       <c r="C41" t="s">
         <v>98</v>
       </c>
+      <c r="D41" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -1685,7 +1742,7 @@
         <v>100</v>
       </c>
       <c r="D42" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1710,7 +1767,7 @@
         <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1723,6 +1780,9 @@
       <c r="C45" t="s">
         <v>107</v>
       </c>
+      <c r="D45" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -1734,6 +1794,9 @@
       <c r="C46" t="s">
         <v>109</v>
       </c>
+      <c r="D46" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -1746,7 +1809,7 @@
         <v>111</v>
       </c>
       <c r="D47" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1771,7 +1834,7 @@
         <v>115</v>
       </c>
       <c r="D49" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1784,6 +1847,9 @@
       <c r="C50" t="s">
         <v>117</v>
       </c>
+      <c r="D50" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -1796,7 +1862,7 @@
         <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1810,7 +1876,7 @@
         <v>121</v>
       </c>
       <c r="D52" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1823,6 +1889,9 @@
       <c r="C53" t="s">
         <v>124</v>
       </c>
+      <c r="D53" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -1835,7 +1904,7 @@
         <v>127</v>
       </c>
       <c r="D54" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1849,7 +1918,7 @@
         <v>130</v>
       </c>
       <c r="D55" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1862,6 +1931,9 @@
       <c r="C56" t="s">
         <v>132</v>
       </c>
+      <c r="D56" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -1873,6 +1945,9 @@
       <c r="C57" t="s">
         <v>134</v>
       </c>
+      <c r="D57" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -1884,6 +1959,9 @@
       <c r="C58" t="s">
         <v>136</v>
       </c>
+      <c r="D58" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -1906,6 +1984,9 @@
       <c r="C60" t="s">
         <v>141</v>
       </c>
+      <c r="D60" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
@@ -1918,7 +1999,7 @@
         <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1931,6 +2012,9 @@
       <c r="C62" t="s">
         <v>145</v>
       </c>
+      <c r="D62" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -1942,6 +2026,9 @@
       <c r="C63" t="s">
         <v>147</v>
       </c>
+      <c r="D63" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -1953,6 +2040,9 @@
       <c r="C64" t="s">
         <v>149</v>
       </c>
+      <c r="D64" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
@@ -1964,6 +2054,9 @@
       <c r="C65" t="s">
         <v>151</v>
       </c>
+      <c r="D65" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
@@ -1975,6 +2068,9 @@
       <c r="C66" t="s">
         <v>153</v>
       </c>
+      <c r="D66" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
@@ -1987,7 +2083,7 @@
         <v>155</v>
       </c>
       <c r="D67" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -2000,6 +2096,9 @@
       <c r="C68" t="s">
         <v>157</v>
       </c>
+      <c r="D68" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -2011,6 +2110,9 @@
       <c r="C69" t="s">
         <v>159</v>
       </c>
+      <c r="D69" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
@@ -2022,6 +2124,9 @@
       <c r="C70" t="s">
         <v>161</v>
       </c>
+      <c r="D70" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
@@ -2033,6 +2138,9 @@
       <c r="C71" t="s">
         <v>163</v>
       </c>
+      <c r="D71" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
@@ -2044,6 +2152,9 @@
       <c r="C72" t="s">
         <v>165</v>
       </c>
+      <c r="D72" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
@@ -2055,6 +2166,9 @@
       <c r="C73" t="s">
         <v>167</v>
       </c>
+      <c r="D73" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -2067,7 +2181,7 @@
         <v>169</v>
       </c>
       <c r="D74" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2080,6 +2194,9 @@
       <c r="C75" t="s">
         <v>172</v>
       </c>
+      <c r="D75" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
@@ -2091,6 +2208,9 @@
       <c r="C76" t="s">
         <v>174</v>
       </c>
+      <c r="D76" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
@@ -2102,6 +2222,9 @@
       <c r="C77" t="s">
         <v>176</v>
       </c>
+      <c r="D77" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -2114,7 +2237,7 @@
         <v>178</v>
       </c>
       <c r="D78" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,7 +2251,7 @@
         <v>180</v>
       </c>
       <c r="D79" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2142,7 +2265,7 @@
         <v>182</v>
       </c>
       <c r="D80" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2156,7 +2279,7 @@
         <v>184</v>
       </c>
       <c r="D81" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2170,7 +2293,7 @@
         <v>186</v>
       </c>
       <c r="D82" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2184,7 +2307,7 @@
         <v>188</v>
       </c>
       <c r="D83" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2198,7 +2321,7 @@
         <v>191</v>
       </c>
       <c r="D84" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2212,7 +2335,7 @@
         <v>193</v>
       </c>
       <c r="D85" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2226,7 +2349,7 @@
         <v>195</v>
       </c>
       <c r="D86" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2240,7 +2363,7 @@
         <v>198</v>
       </c>
       <c r="D87" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2254,7 +2377,7 @@
         <v>200</v>
       </c>
       <c r="D88" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2268,7 +2391,7 @@
         <v>203</v>
       </c>
       <c r="D89" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2281,6 +2404,9 @@
       <c r="C90" t="s">
         <v>205</v>
       </c>
+      <c r="D90" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
@@ -2292,6 +2418,9 @@
       <c r="C91" t="s">
         <v>207</v>
       </c>
+      <c r="D91" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
@@ -2303,6 +2432,9 @@
       <c r="C92" t="s">
         <v>209</v>
       </c>
+      <c r="D92" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
@@ -2326,7 +2458,7 @@
         <v>214</v>
       </c>
       <c r="D94" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2339,6 +2471,9 @@
       <c r="C95" t="s">
         <v>216</v>
       </c>
+      <c r="D95" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
@@ -2350,6 +2485,9 @@
       <c r="C96" t="s">
         <v>218</v>
       </c>
+      <c r="D96" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
@@ -2373,7 +2511,7 @@
         <v>223</v>
       </c>
       <c r="D98" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2387,16 +2525,18 @@
         <v>225</v>
       </c>
       <c r="D99" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C20" r:id="rId1" xr:uid="{8949206C-C373-4757-A0DD-230935D3444E}"/>
     <hyperlink ref="C38" r:id="rId2" xr:uid="{990D16FC-5DDA-42BA-9897-AD855F62ACDF}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{6E498A56-6DD9-4825-A3EE-FEA917E37C16}"/>
+    <hyperlink ref="C10" r:id="rId4" xr:uid="{E39A932F-9A6E-4DE9-8DDB-D8D988FACFAF}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ahora los dobles grados con bibliotecas distintas se detectan correctamente
</commit_message>
<xml_diff>
--- a/Grados_UGR_Centros.xlsx
+++ b/Grados_UGR_Centros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\SyllaBUG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820A49B6-61D4-449A-957E-C4E936BF0B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588B4159-26EC-42B5-A9EC-833EED1BBE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="253">
   <si>
     <t>Grado</t>
   </si>
@@ -763,15 +763,9 @@
     <t>B. Derecho + B. Económicas y Empres.</t>
   </si>
   <si>
-    <t xml:space="preserve">B. Políticas y Sociolog. + </t>
-  </si>
-  <si>
     <t>B. Derecho + B. Políticas y Sociolog.</t>
   </si>
   <si>
-    <t xml:space="preserve">B. Económicas y Empres. + </t>
-  </si>
-  <si>
     <t>B. Ciencias + B. Informática y Telecom.</t>
   </si>
   <si>
@@ -779,6 +773,12 @@
   </si>
   <si>
     <t>B. Filosofía y Letras A + B. Eduación</t>
+  </si>
+  <si>
+    <t>B. Económicas y Empres. + B. Politécnica</t>
+  </si>
+  <si>
+    <t>B. Políticas y Sociolog. + B. Colegio Máximo</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="134" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="134" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,7 +1213,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1241,7 +1241,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1255,7 +1255,7 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1283,7 +1283,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1297,7 +1297,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1339,7 +1339,7 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1353,7 +1353,7 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1367,7 +1367,7 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1381,7 +1381,7 @@
         <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1715,6 +1715,9 @@
       </c>
       <c r="C40" t="s">
         <v>96</v>
+      </c>
+      <c r="D40" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Versión mejorada con instrucciones del SyllaBUG, más estética y más efectiva aunque debe mejorar todavía
</commit_message>
<xml_diff>
--- a/Grados_UGR_Centros.xlsx
+++ b/Grados_UGR_Centros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\SyllaBUG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588B4159-26EC-42B5-A9EC-833EED1BBE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAB83ED-7738-417E-A28D-8141C311AD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="255">
   <si>
     <t>Grado</t>
   </si>
@@ -779,6 +779,12 @@
   </si>
   <si>
     <t>B. Políticas y Sociolog. + B. Colegio Máximo</t>
+  </si>
+  <si>
+    <t>B. Arquitectura</t>
+  </si>
+  <si>
+    <t>B. S. Jerónimo</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="134" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="135" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1976,6 +1982,9 @@
       <c r="C59" t="s">
         <v>139</v>
       </c>
+      <c r="D59" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
@@ -2449,6 +2458,9 @@
       <c r="C93" t="s">
         <v>212</v>
       </c>
+      <c r="D93" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
@@ -2501,6 +2513,9 @@
       </c>
       <c r="C97" t="s">
         <v>221</v>
+      </c>
+      <c r="D97" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Cambio de localización grado en filosofía
</commit_message>
<xml_diff>
--- a/Grados_UGR_Centros.xlsx
+++ b/Grados_UGR_Centros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\SyllaBUG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAB83ED-7738-417E-A28D-8141C311AD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F61E928-A965-406C-AD60-3C9E58BFFCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -733,9 +733,6 @@
     <t>B. PTS</t>
   </si>
   <si>
-    <t>B. Psicología y Letras B</t>
-  </si>
-  <si>
     <t>B. Colegio Máximo</t>
   </si>
   <si>
@@ -769,9 +766,6 @@
     <t>B. Ciencias + B. Informática y Telecom.</t>
   </si>
   <si>
-    <t xml:space="preserve"> B. Informática y Telecom. + B. Económicas y Empres.</t>
-  </si>
-  <si>
     <t>B. Filosofía y Letras A + B. Eduación</t>
   </si>
   <si>
@@ -785,13 +779,19 @@
   </si>
   <si>
     <t>B. S. Jerónimo</t>
+  </si>
+  <si>
+    <t>B. Filosofía y Letras B</t>
+  </si>
+  <si>
+    <t>B. Informática y Telecom. + B. Económicas y Empres.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -808,6 +808,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -849,12 +857,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1158,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="135" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,7 +1214,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1219,7 +1228,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1233,7 +1242,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1247,7 +1256,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1261,7 +1270,7 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1289,7 +1298,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1303,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1330,7 +1339,7 @@
       <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>235</v>
       </c>
     </row>
@@ -1345,7 +1354,7 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1359,7 +1368,7 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1373,7 +1382,7 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1387,7 +1396,7 @@
         <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1527,7 +1536,7 @@
         <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1611,7 +1620,7 @@
         <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1625,7 +1634,7 @@
         <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1639,7 +1648,7 @@
         <v>82</v>
       </c>
       <c r="D34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1653,7 +1662,7 @@
         <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1667,7 +1676,7 @@
         <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1681,7 +1690,7 @@
         <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1723,7 +1732,7 @@
         <v>96</v>
       </c>
       <c r="D40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1737,7 +1746,7 @@
         <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1790,7 +1799,7 @@
         <v>107</v>
       </c>
       <c r="D45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1804,7 +1813,7 @@
         <v>109</v>
       </c>
       <c r="D46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1832,7 +1841,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>114</v>
       </c>
@@ -1846,7 +1855,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>116</v>
       </c>
@@ -1857,10 +1866,10 @@
         <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>118</v>
       </c>
@@ -1874,7 +1883,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>120</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -1902,7 +1911,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>125</v>
       </c>
@@ -1916,7 +1925,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>128</v>
       </c>
@@ -1930,7 +1939,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>131</v>
       </c>
@@ -1944,7 +1953,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>133</v>
       </c>
@@ -1958,7 +1967,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>135</v>
       </c>
@@ -1972,7 +1981,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>137</v>
       </c>
@@ -1983,10 +1992,11 @@
         <v>139</v>
       </c>
       <c r="D59" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>140</v>
       </c>
@@ -2000,7 +2010,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>142</v>
       </c>
@@ -2014,7 +2024,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>144</v>
       </c>
@@ -2028,7 +2038,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -2042,7 +2052,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>148</v>
       </c>
@@ -2053,7 +2063,7 @@
         <v>149</v>
       </c>
       <c r="D64" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2193,7 +2203,7 @@
         <v>169</v>
       </c>
       <c r="D74" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2207,7 +2217,7 @@
         <v>172</v>
       </c>
       <c r="D75" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2221,7 +2231,7 @@
         <v>174</v>
       </c>
       <c r="D76" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2249,7 +2259,7 @@
         <v>178</v>
       </c>
       <c r="D78" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2291,7 +2301,7 @@
         <v>184</v>
       </c>
       <c r="D81" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2333,7 +2343,7 @@
         <v>191</v>
       </c>
       <c r="D84" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2403,7 +2413,7 @@
         <v>203</v>
       </c>
       <c r="D89" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2417,7 +2427,7 @@
         <v>205</v>
       </c>
       <c r="D90" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2431,7 +2441,7 @@
         <v>207</v>
       </c>
       <c r="D91" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2459,7 +2469,7 @@
         <v>212</v>
       </c>
       <c r="D93" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2487,7 +2497,7 @@
         <v>216</v>
       </c>
       <c r="D95" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2515,7 +2525,7 @@
         <v>221</v>
       </c>
       <c r="D97" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Arreglado problema notificado B. Psicología y Letras B
</commit_message>
<xml_diff>
--- a/Grados_UGR_Centros.xlsx
+++ b/Grados_UGR_Centros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\SyllaBUG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F61E928-A965-406C-AD60-3C9E58BFFCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F876ED41-629A-4C89-9754-332A510FBAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -766,9 +766,6 @@
     <t>B. Ciencias + B. Informática y Telecom.</t>
   </si>
   <si>
-    <t>B. Filosofía y Letras A + B. Eduación</t>
-  </si>
-  <si>
     <t>B. Económicas y Empres. + B. Politécnica</t>
   </si>
   <si>
@@ -781,10 +778,13 @@
     <t>B. S. Jerónimo</t>
   </si>
   <si>
-    <t>B. Filosofía y Letras B</t>
-  </si>
-  <si>
     <t>B. Informática y Telecom. + B. Económicas y Empres.</t>
+  </si>
+  <si>
+    <t>B. Filosofía y Letras A + B. Educación</t>
+  </si>
+  <si>
+    <t>B. Psicología y Letras B</t>
   </si>
 </sst>
 </file>
@@ -1169,11 +1169,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="46.5546875" customWidth="1"/>
+    <col min="4" max="4" width="53.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1228,7 +1234,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1270,7 +1276,7 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1298,7 +1304,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1312,7 +1318,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1354,7 +1360,7 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1368,7 +1374,7 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1382,7 +1388,7 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1992,7 +1998,7 @@
         <v>139</v>
       </c>
       <c r="D59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G59" s="3"/>
     </row>
@@ -2063,7 +2069,7 @@
         <v>149</v>
       </c>
       <c r="D64" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2343,7 +2349,7 @@
         <v>191</v>
       </c>
       <c r="D84" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2441,7 +2447,7 @@
         <v>207</v>
       </c>
       <c r="D91" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2469,7 +2475,7 @@
         <v>212</v>
       </c>
       <c r="D93" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2525,7 +2531,7 @@
         <v>221</v>
       </c>
       <c r="D97" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>